<commit_message>
Add 3 more tests for Login page
</commit_message>
<xml_diff>
--- a/Blog-Skeleton/UI.tests/DataDrivenTests/LoginUser.xlsx
+++ b/Blog-Skeleton/UI.tests/DataDrivenTests/LoginUser.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>ID</t>
   </si>
@@ -40,13 +40,25 @@
   </si>
   <si>
     <t>Existing</t>
+  </si>
+  <si>
+    <t>LoginWithoutPassword</t>
+  </si>
+  <si>
+    <t>LoginWithoutEmailAndPassword</t>
+  </si>
+  <si>
+    <t>LoginWithExistingUserButWrongPassword</t>
+  </si>
+  <si>
+    <t>Wrong</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
@@ -75,6 +87,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -134,11 +153,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -150,8 +170,10 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -455,16 +477,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -491,14 +513,52 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
One positive test for Login page
</commit_message>
<xml_diff>
--- a/Blog-Skeleton/UI.tests/DataDrivenTests/LoginUser.xlsx
+++ b/Blog-Skeleton/UI.tests/DataDrivenTests/LoginUser.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SoftUni\QA_Automation\Satsuma\QAProjectRepo\Blog-Skeleton\UI.tests\DataDrivenTests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="16830" windowHeight="6465"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -52,12 +47,18 @@
   </si>
   <si>
     <t>Wrong</t>
+  </si>
+  <si>
+    <t>LoginWithNonExistingUserButValidPassword</t>
+  </si>
+  <si>
+    <t>abv@abv.bg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
@@ -233,7 +234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -268,7 +269,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -477,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -553,11 +554,26 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C4" r:id="rId2"/>
     <hyperlink ref="C5" r:id="rId3"/>
+    <hyperlink ref="C6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Two tests for login page
</commit_message>
<xml_diff>
--- a/Blog-Skeleton/UI.tests/DataDrivenTests/LoginUser.xlsx
+++ b/Blog-Skeleton/UI.tests/DataDrivenTests/LoginUser.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t>abv@abv.bg</t>
+  </si>
+  <si>
+    <t>LoginWithValidPasswordAsEmail</t>
+  </si>
+  <si>
+    <t>LoginWithRandomNumbersAsEmailAndPassword</t>
+  </si>
+  <si>
+    <t>LoginWithInvalidEmail</t>
   </si>
 </sst>
 </file>
@@ -478,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -568,12 +577,49 @@
         <v>6</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>1234</v>
+      </c>
+      <c r="D9">
+        <v>1234</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C4" r:id="rId2"/>
     <hyperlink ref="C5" r:id="rId3"/>
     <hyperlink ref="C6" r:id="rId4"/>
+    <hyperlink ref="C8" r:id="rId5" display="abv@abv.bg"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>